<commit_message>
Add Census Region attribute in segment dropdown
</commit_message>
<xml_diff>
--- a/public/data_dictionary.xlsx
+++ b/public/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irfan\Dropbox (ASU)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibatur/Dropbox (ASU)/irfan_batur/projects/t3_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A498B0E-0A32-4C9C-AE64-6F6F41260E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A740A-F99B-294C-930D-A608128A57AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17835" windowHeight="15585" xr2:uid="{D1670C46-BC23-459B-A4EC-9C6FF771585A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17840" windowHeight="15580" xr2:uid="{D1670C46-BC23-459B-A4EC-9C6FF771585A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>non_metropolitan</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>norm_wb</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>1 = respondent's household located in a non-metrepolitan area; 0 = otherwise</t>
   </si>
   <si>
-    <t>state where respondent's household is located</t>
-  </si>
-  <si>
     <t>daily wellbeing score of respondent (continuous)</t>
   </si>
   <si>
@@ -648,6 +642,12 @@
   </si>
   <si>
     <t>1 = respondent who are employed but reported no work activity on the survey day; 0 = otherwise</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>census region where respondent's household is located; 1 = Northeast; 2 = Midwest; 3 = South; 4 = West</t>
   </si>
 </sst>
 </file>
@@ -1016,886 +1016,886 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FE2E3B-DBEC-4F83-931D-53115C5CDF6C}">
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>120</v>
+      </c>
+      <c r="B79" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>62</v>
+      </c>
+      <c r="B83" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>127</v>
+      </c>
+      <c r="B87" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>128</v>
+      </c>
+      <c r="B89" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>108</v>
+      </c>
+      <c r="B93" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>115</v>
+      </c>
+      <c r="B96" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>111</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>73</v>
       </c>
-      <c r="B36" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>105</v>
-      </c>
-      <c r="B55" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>95</v>
-      </c>
-      <c r="B63" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>96</v>
-      </c>
-      <c r="B64" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>101</v>
-      </c>
-      <c r="B67" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>102</v>
-      </c>
-      <c r="B68" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>103</v>
-      </c>
-      <c r="B69" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>84</v>
-      </c>
-      <c r="B70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>85</v>
-      </c>
-      <c r="B71" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>107</v>
-      </c>
-      <c r="B72" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>106</v>
-      </c>
-      <c r="B73" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>125</v>
-      </c>
-      <c r="B74" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>121</v>
-      </c>
-      <c r="B75" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>124</v>
-      </c>
-      <c r="B76" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>120</v>
-      </c>
-      <c r="B77" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>126</v>
-      </c>
-      <c r="B78" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>122</v>
-      </c>
-      <c r="B79" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B80" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>123</v>
-      </c>
-      <c r="B81" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>119</v>
-      </c>
-      <c r="B82" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>64</v>
-      </c>
-      <c r="B83" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>133</v>
-      </c>
-      <c r="B84" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>134</v>
-      </c>
-      <c r="B85" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>129</v>
-      </c>
-      <c r="B87" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>132</v>
-      </c>
-      <c r="B88" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>130</v>
-      </c>
-      <c r="B89" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>115</v>
-      </c>
-      <c r="B90" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>111</v>
-      </c>
-      <c r="B91" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>114</v>
-      </c>
-      <c r="B92" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>110</v>
-      </c>
-      <c r="B93" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>116</v>
-      </c>
-      <c r="B94" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>112</v>
-      </c>
-      <c r="B95" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>117</v>
-      </c>
-      <c r="B96" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>113</v>
-      </c>
-      <c r="B97" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>109</v>
-      </c>
-      <c r="B98" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>131</v>
-      </c>
-      <c r="B99" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>75</v>
-      </c>
       <c r="B100" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>26</v>
-      </c>
       <c r="B101" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>0</v>
       </c>
       <c r="B102" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B103" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>138</v>
+      </c>
+      <c r="B104" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>133</v>
+      </c>
+      <c r="B105" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>136</v>
+      </c>
+      <c r="B106" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>134</v>
+      </c>
+      <c r="B107" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>140</v>
-      </c>
-      <c r="B104" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>135</v>
+      </c>
+      <c r="B108" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>135</v>
-      </c>
-      <c r="B105" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>138</v>
-      </c>
-      <c r="B106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>136</v>
-      </c>
-      <c r="B107" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>137</v>
-      </c>
-      <c r="B108" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the menu dropdown with Census Division
</commit_message>
<xml_diff>
--- a/public/data_dictionary.xlsx
+++ b/public/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibatur/Dropbox (ASU)/irfan_batur/projects/t3_dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irfan\Dropbox (ASU)\irfan_batur\projects\t3_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A740A-F99B-294C-930D-A608128A57AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EB7290-2065-4044-901F-444CE3A0D968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17840" windowHeight="15580" xr2:uid="{D1670C46-BC23-459B-A4EC-9C6FF771585A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D1670C46-BC23-459B-A4EC-9C6FF771585A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -644,10 +644,10 @@
     <t>1 = respondent who are employed but reported no work activity on the survey day; 0 = otherwise</t>
   </si>
   <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>census region where respondent's household is located; 1 = Northeast; 2 = Midwest; 3 = South; 4 = West</t>
+    <t>division</t>
+  </si>
+  <si>
+    <t>census division where respondent's household is located; 1 = new england; 2 = middle atlantic; 3 = east north central; 4 = west north central; 5 = south atlantic; 6 = east south central; 7 = west south central; 8 = mountain; 9 = pacific</t>
   </si>
 </sst>
 </file>
@@ -697,9 +697,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,17 +1022,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FE2E3B-DBEC-4F83-931D-53115C5CDF6C}">
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1258,7 +1264,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1290,7 +1296,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>126</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -1386,7 +1392,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1394,7 +1400,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -1434,7 +1440,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>78</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -1482,7 +1488,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>96</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -1498,7 +1504,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -1514,7 +1520,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>92</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>93</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>94</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>95</v>
       </c>
@@ -1546,7 +1552,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -1554,7 +1560,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>99</v>
       </c>
@@ -1562,7 +1568,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -1570,7 +1576,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -1586,7 +1592,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>105</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>104</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>123</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>119</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>122</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>118</v>
       </c>
@@ -1642,7 +1648,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>124</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>120</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>125</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>121</v>
       </c>
@@ -1674,7 +1680,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>117</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>62</v>
       </c>
@@ -1690,7 +1696,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>131</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>132</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>127</v>
       </c>
@@ -1722,7 +1728,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>130</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>128</v>
       </c>
@@ -1738,7 +1744,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>113</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>109</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>112</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -1770,7 +1776,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>114</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>129</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>73</v>
       </c>
@@ -1826,15 +1832,15 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+    <row r="101" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>137</v>
       </c>
@@ -1850,7 +1856,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>138</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>133</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>136</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>134</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>135</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>116</v>
       </c>

</xml_diff>